<commit_message>
Update: all latest data & script 1 Auguts 2025
</commit_message>
<xml_diff>
--- a/data/Anomaly_Growth_KabKec.xlsx
+++ b/data/Anomaly_Growth_KabKec.xlsx
@@ -3971,7 +3971,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-06-27</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -4018,12 +4018,12 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-06-27</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>After MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H76" t="n">
@@ -9564,12 +9564,12 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H194" t="n">
@@ -9611,12 +9611,12 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H195" t="n">
@@ -9658,12 +9658,12 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H196" t="n">
@@ -9705,12 +9705,12 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H197" t="n">
@@ -9752,12 +9752,12 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H198" t="n">
@@ -9799,12 +9799,12 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H199" t="n">
@@ -17272,7 +17272,7 @@
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G358" t="inlineStr">
@@ -17319,7 +17319,7 @@
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G359" t="inlineStr">
@@ -17366,7 +17366,7 @@
       </c>
       <c r="F360" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G360" t="inlineStr">
@@ -17413,7 +17413,7 @@
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G361" t="inlineStr">
@@ -25544,7 +25544,7 @@
       </c>
       <c r="F534" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G534" t="inlineStr">
@@ -25591,7 +25591,7 @@
       </c>
       <c r="F535" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G535" t="inlineStr">
@@ -25638,7 +25638,7 @@
       </c>
       <c r="F536" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G536" t="inlineStr">
@@ -25685,7 +25685,7 @@
       </c>
       <c r="F537" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G537" t="inlineStr">
@@ -33158,12 +33158,12 @@
       </c>
       <c r="F696" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G696" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H696" t="n">
@@ -33205,12 +33205,12 @@
       </c>
       <c r="F697" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G697" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H697" t="n">
@@ -33252,12 +33252,12 @@
       </c>
       <c r="F698" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G698" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H698" t="n">
@@ -33299,12 +33299,12 @@
       </c>
       <c r="F699" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G699" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H699" t="n">
@@ -33346,12 +33346,12 @@
       </c>
       <c r="F700" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G700" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H700" t="n">
@@ -37106,12 +37106,12 @@
       </c>
       <c r="F780" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G780" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H780" t="n">
@@ -37153,12 +37153,12 @@
       </c>
       <c r="F781" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G781" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H781" t="n">
@@ -37200,12 +37200,12 @@
       </c>
       <c r="F782" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G782" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H782" t="n">
@@ -37247,12 +37247,12 @@
       </c>
       <c r="F783" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G783" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H783" t="n">
@@ -41289,12 +41289,12 @@
       </c>
       <c r="F869" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G869" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H869" t="n">
@@ -41336,12 +41336,12 @@
       </c>
       <c r="F870" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G870" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H870" t="n">
@@ -41383,12 +41383,12 @@
       </c>
       <c r="F871" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G871" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H871" t="n">
@@ -41430,12 +41430,12 @@
       </c>
       <c r="F872" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G872" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H872" t="n">
@@ -50548,7 +50548,7 @@
       </c>
       <c r="F1066" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1066" t="inlineStr">
@@ -50595,7 +50595,7 @@
       </c>
       <c r="F1067" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1067" t="inlineStr">
@@ -50642,7 +50642,7 @@
       </c>
       <c r="F1068" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1068" t="inlineStr">
@@ -50689,7 +50689,7 @@
       </c>
       <c r="F1069" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1069" t="inlineStr">
@@ -50736,7 +50736,7 @@
       </c>
       <c r="F1070" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1070" t="inlineStr">
@@ -50783,7 +50783,7 @@
       </c>
       <c r="F1071" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1071" t="inlineStr">
@@ -68737,12 +68737,12 @@
       </c>
       <c r="F1453" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1453" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1453" t="n">
@@ -68784,12 +68784,12 @@
       </c>
       <c r="F1454" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1454" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1454" t="n">
@@ -68831,12 +68831,12 @@
       </c>
       <c r="F1455" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1455" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1455" t="n">
@@ -68878,12 +68878,12 @@
       </c>
       <c r="F1456" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1456" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1456" t="n">
@@ -68925,12 +68925,12 @@
       </c>
       <c r="F1457" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1457" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1457" t="n">
@@ -74847,12 +74847,12 @@
       </c>
       <c r="F1583" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1583" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1583" t="n">
@@ -74894,12 +74894,12 @@
       </c>
       <c r="F1584" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1584" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1584" t="n">
@@ -74941,12 +74941,12 @@
       </c>
       <c r="F1585" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1585" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1585" t="n">
@@ -74988,12 +74988,12 @@
       </c>
       <c r="F1586" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1586" t="inlineStr">
         <is>
-          <t>NY MOCN</t>
+          <t>Before MOCN</t>
         </is>
       </c>
       <c r="H1586" t="n">
@@ -75317,7 +75317,7 @@
       </c>
       <c r="F1593" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1593" t="inlineStr">
@@ -75364,7 +75364,7 @@
       </c>
       <c r="F1594" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1594" t="inlineStr">
@@ -75411,7 +75411,7 @@
       </c>
       <c r="F1595" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1595" t="inlineStr">
@@ -75458,7 +75458,7 @@
       </c>
       <c r="F1596" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1596" t="inlineStr">
@@ -75505,7 +75505,7 @@
       </c>
       <c r="F1597" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-07-31</t>
         </is>
       </c>
       <c r="G1597" t="inlineStr">
@@ -78077,7 +78077,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -78251,26 +78251,17 @@
           <t>KAB. BANDUNG BARAT</t>
         </is>
       </c>
-      <c r="B6" s="5" t="n">
-        <v>0.09640076633610818</v>
-      </c>
+      <c r="B6" s="6" t="inlineStr"/>
       <c r="C6" s="5" t="n">
         <v>0.01793758449584748</v>
       </c>
-      <c r="D6" s="5" t="n">
-        <v>0.1137235598808345</v>
-      </c>
+      <c r="D6" s="6" t="inlineStr"/>
       <c r="E6" s="5" t="n">
         <v>0.07035073453796234</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-06-28_2025-07-04</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -78411,20 +78402,20 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KAB. BENGKULU SELATAN</t>
+          <t>KAB. BENGKAYANG</t>
         </is>
       </c>
       <c r="B11" s="6" t="inlineStr"/>
       <c r="C11" s="4" t="n">
-        <v>-0.1147333139779707</v>
+        <v>-0.1007308328014116</v>
       </c>
       <c r="D11" s="6" t="inlineStr"/>
       <c r="E11" s="5" t="n">
-        <v>2.94934611898938</v>
+        <v>0.6494484532780436</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
+          <t>2025-05-20_2025-05-26</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -78436,16 +78427,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KAB. BOJONEGORO</t>
+          <t>KAB. BENGKULU SELATAN</t>
         </is>
       </c>
       <c r="B12" s="6" t="inlineStr"/>
       <c r="C12" s="4" t="n">
-        <v>-0.07678683688516738</v>
+        <v>-0.1147333139779707</v>
       </c>
       <c r="D12" s="6" t="inlineStr"/>
-      <c r="E12" s="4" t="n">
-        <v>-0.01191368790837241</v>
+      <c r="E12" s="5" t="n">
+        <v>2.94934611898938</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -78454,70 +78445,61 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-07-23_2025-07-29</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KAB. BOMBANA</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>-0.02326244641072626</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>0.0839540829976814</v>
-      </c>
-      <c r="D13" s="5" t="n">
-        <v>2.427809798717411</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>5.190847734802833</v>
+          <t>KAB. BOJONEGORO</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr"/>
+      <c r="C13" s="4" t="n">
+        <v>-0.07678683688516738</v>
+      </c>
+      <c r="D13" s="6" t="inlineStr"/>
+      <c r="E13" s="4" t="n">
+        <v>-0.01191368790837241</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-21_2025-05-27</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2025-06-14_2025-06-20</t>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-23_2025-07-29</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>KAB. BONE</t>
+          <t>KAB. BOMBANA</t>
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>-0.05807891421917123</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>-0.05807891421917123</v>
+        <v>-0.02326244641072626</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>0.0839540829976814</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.06452210503891556</v>
+        <v>2.427809798717411</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.06452210503891556</v>
+        <v>5.190847734802833</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
+          <t>2025-05-21_2025-05-27</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-06-14_2025-06-20</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -78529,20 +78511,20 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>KAB. BULUKUMBA</t>
+          <t>KAB. BONE</t>
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>-0.01319251776984156</v>
+        <v>-0.05807891421917123</v>
       </c>
       <c r="C15" s="4" t="n">
-        <v>-0.05311914442516537</v>
+        <v>-0.05807891421917123</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.002592696509341021</v>
+        <v>0.06452210503891556</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1293181275456221</v>
+        <v>0.06452210503891556</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -78551,7 +78533,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-22_2025-05-28</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -78563,29 +78545,29 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>KAB. BULUNGAN</t>
+          <t>KAB. BULUKUMBA</t>
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>-0.07463980277087587</v>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>0.01515691038651186</v>
+        <v>-0.01319251776984156</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>-0.05311914442516537</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>4.559988230295124</v>
+        <v>0.002592696509341021</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>11.18086736471109</v>
+        <v>0.1293181275456221</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-16_2025-05-22</t>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-07-12_2025-07-18</t>
+          <t>2025-05-22_2025-05-28</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -78597,20 +78579,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>KAB. GIANYAR</t>
-        </is>
-      </c>
-      <c r="B17" s="6" t="inlineStr"/>
+          <t>KAB. BULUNGAN</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>-0.07463980277087587</v>
+      </c>
       <c r="C17" s="5" t="n">
-        <v>0.02112525161233228</v>
-      </c>
-      <c r="D17" s="6" t="inlineStr"/>
+        <v>0.01515691038651186</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>4.559988230295124</v>
+      </c>
       <c r="E17" s="5" t="n">
-        <v>0.154469092923176</v>
+        <v>11.18086736471109</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-18_2025-05-24</t>
+          <t>2025-05-16_2025-05-22</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-07-12_2025-07-18</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -78622,29 +78613,20 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>KAB. GUNUNGKIDUL</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="n">
-        <v>-0.03401706367631925</v>
-      </c>
-      <c r="C18" s="4" t="n">
-        <v>-0.07793120627323701</v>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v>0.06294650756199516</v>
-      </c>
+          <t>KAB. GIANYAR</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr"/>
+      <c r="C18" s="5" t="n">
+        <v>0.02112525161233228</v>
+      </c>
+      <c r="D18" s="6" t="inlineStr"/>
       <c r="E18" s="5" t="n">
-        <v>0.0642753907214543</v>
+        <v>0.154469092923176</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2025-06-14_2025-06-20</t>
+          <t>2025-05-18_2025-05-24</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -78656,20 +78638,20 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>KAB. JENEPONTO</t>
+          <t>KAB. GUNUNGKIDUL</t>
         </is>
       </c>
       <c r="B19" s="4" t="n">
-        <v>-0.1152823520380198</v>
+        <v>-0.03401706367631925</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>-0.1776616389372345</v>
+        <v>-0.07793120627323701</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.3116275374495908</v>
+        <v>0.06294650756199516</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.2568072270953821</v>
+        <v>0.0642753907214543</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -78678,7 +78660,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-07-01_2025-07-07</t>
+          <t>2025-06-14_2025-06-20</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -78690,20 +78672,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KAB. KAUR</t>
-        </is>
-      </c>
-      <c r="B20" s="5" t="n">
-        <v>0.06119934124913295</v>
+          <t>KAB. JENEPONTO</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>-0.1152823520380198</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>-0.01512924760145481</v>
+        <v>-0.1776616389372345</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>3.574669856722226</v>
+        <v>0.3116275374495908</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>6.50313284446292</v>
+        <v>0.2568072270953821</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -78712,7 +78694,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-06-30_2025-07-06</t>
+          <t>2025-07-01_2025-07-07</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -78724,20 +78706,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>KAB. KENDAL</t>
-        </is>
-      </c>
-      <c r="B21" s="6" t="inlineStr"/>
+          <t>KAB. KAUR</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>0.06119934124913295</v>
+      </c>
       <c r="C21" s="4" t="n">
-        <v>-0.1727869135549594</v>
-      </c>
-      <c r="D21" s="6" t="inlineStr"/>
-      <c r="E21" s="4" t="n">
-        <v>-0.3801520675920409</v>
+        <v>-0.01512924760145481</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>3.574669856722226</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>6.50313284446292</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-06-30_2025-07-06</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -78749,29 +78740,20 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>KAB. KLATEN</t>
-        </is>
-      </c>
-      <c r="B22" s="4" t="n">
-        <v>-0.06829135616837755</v>
-      </c>
+          <t>KAB. KENDAL</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr"/>
       <c r="C22" s="4" t="n">
-        <v>-0.08601074200150785</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <v>0.07935376995374623</v>
-      </c>
-      <c r="E22" s="5" t="n">
-        <v>0.05607504110239849</v>
+        <v>-0.1727869135549594</v>
+      </c>
+      <c r="D22" s="6" t="inlineStr"/>
+      <c r="E22" s="4" t="n">
+        <v>-0.3801520675920409</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2025-06-19_2025-06-25</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -78783,20 +78765,20 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>KAB. KLUNGKUNG</t>
+          <t>KAB. KLATEN</t>
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>-0.06132508680190375</v>
+        <v>-0.06829135616837755</v>
       </c>
       <c r="C23" s="4" t="n">
-        <v>-0.0666202570704176</v>
+        <v>-0.08601074200150785</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0.194058415123839</v>
+        <v>0.07935376995374623</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0.1934392894952084</v>
+        <v>0.05607504110239849</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -78805,7 +78787,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-07-22_2025-07-28</t>
+          <t>2025-06-19_2025-06-25</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -78817,20 +78799,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>KAB. KOLAKA</t>
-        </is>
-      </c>
-      <c r="B24" s="6" t="inlineStr"/>
-      <c r="C24" s="5" t="n">
-        <v>0.01334624519846942</v>
-      </c>
-      <c r="D24" s="6" t="inlineStr"/>
+          <t>KAB. KLUNGKUNG</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>-0.06132508680190375</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>-0.0666202570704176</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.194058415123839</v>
+      </c>
       <c r="E24" s="5" t="n">
-        <v>12.89836123198442</v>
+        <v>0.1934392894952084</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-13_2025-05-19</t>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-07-22_2025-07-28</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -78842,16 +78833,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>KAB. KOLAKA TIMUR</t>
+          <t>KAB. KOLAKA</t>
         </is>
       </c>
       <c r="B25" s="6" t="inlineStr"/>
       <c r="C25" s="5" t="n">
-        <v>0.08670800526641374</v>
+        <v>0.01334624519846942</v>
       </c>
       <c r="D25" s="6" t="inlineStr"/>
       <c r="E25" s="5" t="n">
-        <v>20.12867852517187</v>
+        <v>12.89836123198442</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -78867,29 +78858,20 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>KAB. KONAWE</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>-0.001334581859731163</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>-0.03404498924256469</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <v>25.70697833646306</v>
-      </c>
+          <t>KAB. KOLAKA TIMUR</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr"/>
+      <c r="C26" s="5" t="n">
+        <v>0.08670800526641374</v>
+      </c>
+      <c r="D26" s="6" t="inlineStr"/>
       <c r="E26" s="5" t="n">
-        <v>30.56591151521785</v>
+        <v>20.12867852517187</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>2025-05-13_2025-05-19</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2025-07-13_2025-07-19</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -78901,29 +78883,29 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>KAB. KONAWE KEPULAUAN</t>
-        </is>
-      </c>
-      <c r="B27" s="5" t="n">
-        <v>0.03272664810596324</v>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>0.1437388861887125</v>
+          <t>KAB. KONAWE</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>-0.001334581859731163</v>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>-0.03404498924256469</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>3.813903379416232</v>
+        <v>25.70697833646306</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>4.959332808684576</v>
+        <v>30.56591151521785</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-23_2025-05-29</t>
+          <t>2025-05-13_2025-05-19</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-07-08_2025-07-14</t>
+          <t>2025-07-13_2025-07-19</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -78935,29 +78917,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>KAB. KONAWE SELATAN</t>
-        </is>
-      </c>
-      <c r="B28" s="4" t="n">
-        <v>-0.02772340061340307</v>
-      </c>
-      <c r="C28" s="4" t="n">
-        <v>-0.006006768597992873</v>
+          <t>KAB. KONAWE KEPULAUAN</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>0.03272664810596324</v>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>0.1437388861887125</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>30.60588301865913</v>
+        <v>3.813903379416232</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>41.09534589223921</v>
+        <v>4.959332808684576</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-13_2025-05-19</t>
+          <t>2025-05-23_2025-05-29</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-06-30_2025-07-06</t>
+          <t>2025-07-08_2025-07-14</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -78969,75 +78951,84 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>KAB. KUTAI BARAT</t>
-        </is>
-      </c>
-      <c r="B29" s="5" t="n">
-        <v>0.2152087940824503</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>0.1793289755984087</v>
+          <t>KAB. KONAWE SELATAN</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>-0.02772340061340307</v>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>-0.006006768597992873</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>10.6740504779404</v>
+        <v>30.60588301865913</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>10.3149202545403</v>
+        <v>41.09534589223921</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-16_2025-05-22</t>
+          <t>2025-05-13_2025-05-19</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-07-21_2025-07-27</t>
+          <t>2025-06-30_2025-07-06</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-07-23_2025-07-29</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>KAB. KUTAI KARTANEGARA</t>
-        </is>
-      </c>
-      <c r="B30" s="6" t="inlineStr"/>
+          <t>KAB. KUTAI BARAT</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>0.2152087940824503</v>
+      </c>
       <c r="C30" s="5" t="n">
-        <v>0.005840108239291522</v>
-      </c>
-      <c r="D30" s="6" t="inlineStr"/>
+        <v>0.1793289755984087</v>
+      </c>
+      <c r="D30" s="5" t="n">
+        <v>10.6740504779404</v>
+      </c>
       <c r="E30" s="5" t="n">
-        <v>0.3567266386788076</v>
+        <v>10.3149202545403</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
+          <t>2025-05-16_2025-05-22</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-07-21_2025-07-27</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-23_2025-07-29</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>KAB. LABUHANBATU</t>
+          <t>KAB. KUTAI KARTANEGARA</t>
         </is>
       </c>
       <c r="B31" s="6" t="inlineStr"/>
-      <c r="C31" s="4" t="n">
-        <v>-0.1442386489020899</v>
+      <c r="C31" s="5" t="n">
+        <v>0.005840108239291522</v>
       </c>
       <c r="D31" s="6" t="inlineStr"/>
       <c r="E31" s="5" t="n">
-        <v>0.5250260531212306</v>
+        <v>0.3567266386788076</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -79053,29 +79044,20 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>KAB. LABUHANBATU SELATAN</t>
-        </is>
-      </c>
-      <c r="B32" s="4" t="n">
-        <v>-0.2335650795574124</v>
-      </c>
+          <t>KAB. LABUHANBATU</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="inlineStr"/>
       <c r="C32" s="4" t="n">
-        <v>-0.2710851273563264</v>
-      </c>
-      <c r="D32" s="5" t="n">
-        <v>0.5359978241058273</v>
-      </c>
+        <v>-0.1442386489020899</v>
+      </c>
+      <c r="D32" s="6" t="inlineStr"/>
       <c r="E32" s="5" t="n">
-        <v>0.6810598057074276</v>
+        <v>0.5250260531212306</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2025-07-07_2025-07-13</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -79087,20 +79069,20 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>KAB. LABUHANBATU UTARA</t>
+          <t>KAB. LABUHANBATU SELATAN</t>
         </is>
       </c>
       <c r="B33" s="4" t="n">
-        <v>-0.1538630979929346</v>
+        <v>-0.2335650795574124</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>-0.1753279798625644</v>
+        <v>-0.2710851273563264</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>0.384300064119827</v>
+        <v>0.5359978241058273</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>0.3929064971476554</v>
+        <v>0.6810598057074276</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -79109,7 +79091,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-07-20_2025-07-26</t>
+          <t>2025-07-07_2025-07-13</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -79121,20 +79103,20 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>KAB. LAHAT</t>
-        </is>
-      </c>
-      <c r="B34" s="5" t="n">
-        <v>0.03441340077485824</v>
+          <t>KAB. LABUHANBATU UTARA</t>
+        </is>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>-0.1538630979929346</v>
       </c>
       <c r="C34" s="4" t="n">
-        <v>-0.03217035546307517</v>
+        <v>-0.1753279798625644</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>0.005245456695713763</v>
-      </c>
-      <c r="E34" s="4" t="n">
-        <v>-0.006123214894978389</v>
+        <v>0.384300064119827</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>0.3929064971476554</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -79143,7 +79125,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-06-29_2025-07-05</t>
+          <t>2025-07-20_2025-07-26</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -79155,29 +79137,29 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>KAB. LAMANDAU</t>
-        </is>
-      </c>
-      <c r="B35" s="4" t="n">
-        <v>-0.1284316001078134</v>
+          <t>KAB. LAHAT</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>0.03441340077485824</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>-0.168370916151586</v>
+        <v>-0.03217035546307517</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>3.021310351801893</v>
-      </c>
-      <c r="E35" s="5" t="n">
-        <v>6.741256735733494</v>
+        <v>0.005245456695713763</v>
+      </c>
+      <c r="E35" s="4" t="n">
+        <v>-0.006123214894978389</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-16_2025-05-22</t>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-06-27_2025-07-03</t>
+          <t>2025-06-29_2025-07-05</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -79189,20 +79171,29 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>KAB. LAMPUNG BARAT</t>
-        </is>
-      </c>
-      <c r="B36" s="6" t="inlineStr"/>
-      <c r="C36" s="5" t="n">
-        <v>0.07278006844157665</v>
-      </c>
-      <c r="D36" s="6" t="inlineStr"/>
+          <t>KAB. LAMANDAU</t>
+        </is>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>-0.1284316001078134</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>-0.168370916151586</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <v>3.021310351801893</v>
+      </c>
       <c r="E36" s="5" t="n">
-        <v>1.672726452439722</v>
+        <v>6.741256735733494</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
+          <t>2025-05-16_2025-05-22</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -79214,29 +79205,20 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>KAB. MALINAU</t>
-        </is>
-      </c>
-      <c r="B37" s="5" t="n">
-        <v>0.1464237797915809</v>
-      </c>
+          <t>KAB. LAMPUNG BARAT</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr"/>
       <c r="C37" s="5" t="n">
-        <v>0.1583872127104695</v>
-      </c>
-      <c r="D37" s="5" t="n">
-        <v>9.469940173594104</v>
-      </c>
+        <v>0.07278006844157665</v>
+      </c>
+      <c r="D37" s="6" t="inlineStr"/>
       <c r="E37" s="5" t="n">
-        <v>13.74216250162421</v>
+        <v>1.672726452439722</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-16_2025-05-22</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2025-06-30_2025-07-06</t>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -79248,54 +79230,54 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>KAB. MANDAILING NATAL</t>
-        </is>
-      </c>
-      <c r="B38" s="5" t="n">
-        <v>0.02395374884734611</v>
-      </c>
+          <t>KAB. LOMBOK TENGAH</t>
+        </is>
+      </c>
+      <c r="B38" s="6" t="inlineStr"/>
       <c r="C38" s="4" t="n">
-        <v>-0.0211578295124839</v>
-      </c>
-      <c r="D38" s="5" t="n">
-        <v>2.177274339771607</v>
-      </c>
+        <v>-0.08394568799837453</v>
+      </c>
+      <c r="D38" s="6" t="inlineStr"/>
       <c r="E38" s="5" t="n">
-        <v>2.249610465252045</v>
+        <v>0.1420998392571284</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>2025-06-27_2025-07-03</t>
+          <t>2025-05-18_2025-05-24</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-07-18_2025-07-24</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>KAB. MEMPAWAH</t>
-        </is>
-      </c>
-      <c r="B39" s="6" t="inlineStr"/>
-      <c r="C39" s="4" t="n">
-        <v>-0.04291320685544057</v>
-      </c>
-      <c r="D39" s="6" t="inlineStr"/>
-      <c r="E39" s="4" t="n">
-        <v>-0.009782144383831943</v>
+          <t>KAB. MALINAU</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>0.1464237797915809</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>0.1583872127104695</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <v>9.469940173594104</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>13.74216250162421</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
+          <t>2025-05-16_2025-05-22</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-06-30_2025-07-06</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -79307,41 +79289,50 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>KAB. MUARA ENIM</t>
-        </is>
-      </c>
-      <c r="B40" s="6" t="inlineStr"/>
+          <t>KAB. MANDAILING NATAL</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>0.02395374884734611</v>
+      </c>
       <c r="C40" s="4" t="n">
-        <v>-0.03208060385429735</v>
-      </c>
-      <c r="D40" s="6" t="inlineStr"/>
+        <v>-0.0211578295124839</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <v>2.177274339771607</v>
+      </c>
       <c r="E40" s="5" t="n">
-        <v>0.03739995892711013</v>
+        <v>2.249610465252045</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-06-27_2025-07-03</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-18_2025-07-24</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>KAB. NGAWI</t>
+          <t>KAB. MAROS</t>
         </is>
       </c>
       <c r="B41" s="6" t="inlineStr"/>
       <c r="C41" s="4" t="n">
-        <v>-0.0699581391435645</v>
+        <v>-0.01244473647466486</v>
       </c>
       <c r="D41" s="6" t="inlineStr"/>
-      <c r="E41" s="4" t="n">
-        <v>-0.01958142480220236</v>
+      <c r="E41" s="5" t="n">
+        <v>0.02289691815486469</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -79357,29 +79348,20 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>KAB. OGAN KOMERING ULU</t>
-        </is>
-      </c>
-      <c r="B42" s="5" t="n">
-        <v>0.03182370628595597</v>
-      </c>
+          <t>KAB. MEMPAWAH</t>
+        </is>
+      </c>
+      <c r="B42" s="6" t="inlineStr"/>
       <c r="C42" s="4" t="n">
-        <v>-0.03371052362953161</v>
-      </c>
-      <c r="D42" s="5" t="n">
-        <v>0.006702597058948098</v>
-      </c>
-      <c r="E42" s="5" t="n">
-        <v>0.04576049723732269</v>
+        <v>-0.04291320685544057</v>
+      </c>
+      <c r="D42" s="6" t="inlineStr"/>
+      <c r="E42" s="4" t="n">
+        <v>-0.009782144383831943</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -79391,20 +79373,20 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>KAB. OGAN KOMERING ULU SELATAN</t>
-        </is>
-      </c>
-      <c r="B43" s="5" t="n">
-        <v>0.1051969810713825</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>0.04889345317463406</v>
+          <t>KAB. MUARA ENIM</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr"/>
+      <c r="C43" s="4" t="n">
+        <v>-0.03208060385429735</v>
       </c>
       <c r="D43" s="6" t="inlineStr"/>
-      <c r="E43" s="6" t="inlineStr"/>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2025-07-01_2025-07-07</t>
+      <c r="E43" s="5" t="n">
+        <v>0.03739995892711013</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -79416,20 +79398,20 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>KAB. PADANG LAWAS</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="n">
-        <v>-0.1780340896595287</v>
-      </c>
+          <t>KAB. MUSI RAWAS</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="inlineStr"/>
       <c r="C44" s="4" t="n">
-        <v>-0.2566891536833055</v>
+        <v>-0.04624205472512451</v>
       </c>
       <c r="D44" s="6" t="inlineStr"/>
-      <c r="E44" s="6" t="inlineStr"/>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>2025-06-27_2025-07-03</t>
+      <c r="E44" s="5" t="n">
+        <v>0.3271075010382557</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -79441,20 +79423,20 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>KAB. PADANG LAWAS UTARA</t>
-        </is>
-      </c>
-      <c r="B45" s="4" t="n">
-        <v>-0.2381234238696407</v>
-      </c>
+          <t>KAB. NGAWI</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr"/>
       <c r="C45" s="4" t="n">
-        <v>-0.2200030362045176</v>
+        <v>-0.0699581391435645</v>
       </c>
       <c r="D45" s="6" t="inlineStr"/>
-      <c r="E45" s="6" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>2025-07-15_2025-07-21</t>
+      <c r="E45" s="4" t="n">
+        <v>-0.01958142480220236</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -79466,20 +79448,29 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>KAB. PADANG PARIAMAN</t>
-        </is>
-      </c>
-      <c r="B46" s="6" t="inlineStr"/>
+          <t>KAB. OGAN KOMERING ULU</t>
+        </is>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>0.03182370628595597</v>
+      </c>
       <c r="C46" s="4" t="n">
-        <v>-0.02500827934880021</v>
-      </c>
-      <c r="D46" s="6" t="inlineStr"/>
+        <v>-0.03371052362953161</v>
+      </c>
+      <c r="D46" s="5" t="n">
+        <v>0.006702597058948098</v>
+      </c>
       <c r="E46" s="5" t="n">
-        <v>0.02280780649841248</v>
+        <v>0.04576049723732269</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -79491,29 +79482,20 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>KAB. PAMEKASAN</t>
-        </is>
-      </c>
-      <c r="B47" s="4" t="n">
-        <v>-0.0536931506722742</v>
-      </c>
-      <c r="C47" s="4" t="n">
-        <v>-0.03889957514054453</v>
-      </c>
-      <c r="D47" s="5" t="n">
-        <v>0.3788267748200115</v>
-      </c>
-      <c r="E47" s="5" t="n">
-        <v>0.6556047491837055</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
+          <t>KAB. OGAN KOMERING ULU SELATAN</t>
+        </is>
+      </c>
+      <c r="B47" s="5" t="n">
+        <v>0.1051969810713825</v>
+      </c>
+      <c r="C47" s="5" t="n">
+        <v>0.04889345317463406</v>
+      </c>
+      <c r="D47" s="6" t="inlineStr"/>
+      <c r="E47" s="6" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-06-27_2025-07-03</t>
+          <t>2025-07-01_2025-07-07</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -79525,20 +79507,20 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>KAB. PASAMAN</t>
-        </is>
-      </c>
-      <c r="B48" s="5" t="n">
-        <v>0.06984474719378296</v>
+          <t>KAB. PADANG LAWAS</t>
+        </is>
+      </c>
+      <c r="B48" s="4" t="n">
+        <v>-0.1780340896595287</v>
       </c>
       <c r="C48" s="4" t="n">
-        <v>-0.006173767545828318</v>
+        <v>-0.2566891536833055</v>
       </c>
       <c r="D48" s="6" t="inlineStr"/>
       <c r="E48" s="6" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-06-30_2025-07-06</t>
+          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -79550,29 +79532,20 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>KAB. PASAMAN BARAT</t>
-        </is>
-      </c>
-      <c r="B49" s="5" t="n">
-        <v>0.06465591533300589</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>0.02166454397363704</v>
-      </c>
-      <c r="D49" s="5" t="n">
-        <v>0.0449824981561958</v>
-      </c>
-      <c r="E49" s="4" t="n">
-        <v>-0.01007422180378171</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
+          <t>KAB. PADANG LAWAS UTARA</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="n">
+        <v>-0.2381234238696407</v>
+      </c>
+      <c r="C49" s="4" t="n">
+        <v>-0.2200030362045176</v>
+      </c>
+      <c r="D49" s="6" t="inlineStr"/>
+      <c r="E49" s="6" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-06-11_2025-06-17</t>
+          <t>2025-07-15_2025-07-21</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -79584,29 +79557,20 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>KAB. PESISIR BARAT</t>
-        </is>
-      </c>
-      <c r="B50" s="5" t="n">
-        <v>0.110202574420141</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>0.03767220983938128</v>
-      </c>
-      <c r="D50" s="5" t="n">
-        <v>1.696163704626156</v>
-      </c>
+          <t>KAB. PADANG PARIAMAN</t>
+        </is>
+      </c>
+      <c r="B50" s="6" t="inlineStr"/>
+      <c r="C50" s="4" t="n">
+        <v>-0.02500827934880021</v>
+      </c>
+      <c r="D50" s="6" t="inlineStr"/>
       <c r="E50" s="5" t="n">
-        <v>1.805049403264653</v>
+        <v>0.02280780649841248</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>2025-06-24_2025-06-30</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -79618,54 +79582,54 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>KAB. SAMBAS</t>
-        </is>
-      </c>
-      <c r="B51" s="6" t="inlineStr"/>
+          <t>KAB. PAMEKASAN</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="n">
+        <v>-0.0536931506722742</v>
+      </c>
       <c r="C51" s="4" t="n">
-        <v>-0.07023693687968006</v>
-      </c>
-      <c r="D51" s="6" t="inlineStr"/>
+        <v>-0.03889957514054453</v>
+      </c>
+      <c r="D51" s="5" t="n">
+        <v>0.3788267748200115</v>
+      </c>
       <c r="E51" s="5" t="n">
-        <v>0.5806279775517019</v>
+        <v>0.6556047491837055</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-06-27_2025-07-03</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-07-20_2025-07-26</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>KAB. SAMPANG</t>
-        </is>
-      </c>
-      <c r="B52" s="4" t="n">
-        <v>-0.1343411376228456</v>
+          <t>KAB. PASAMAN</t>
+        </is>
+      </c>
+      <c r="B52" s="5" t="n">
+        <v>0.06984474719378296</v>
       </c>
       <c r="C52" s="4" t="n">
-        <v>-0.06939344128566347</v>
-      </c>
-      <c r="D52" s="5" t="n">
-        <v>0.187785854895615</v>
-      </c>
-      <c r="E52" s="5" t="n">
-        <v>0.2510251813419085</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
+        <v>-0.006173767545828318</v>
+      </c>
+      <c r="D52" s="6" t="inlineStr"/>
+      <c r="E52" s="6" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-07-02_2025-07-08</t>
+          <t>2025-06-30_2025-07-06</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -79677,20 +79641,20 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>KAB. SERANG</t>
-        </is>
-      </c>
-      <c r="B53" s="4" t="n">
-        <v>-0.07504590833602121</v>
-      </c>
-      <c r="C53" s="4" t="n">
-        <v>-0.05455638576395258</v>
+          <t>KAB. PASAMAN BARAT</t>
+        </is>
+      </c>
+      <c r="B53" s="5" t="n">
+        <v>0.06465591533300589</v>
+      </c>
+      <c r="C53" s="5" t="n">
+        <v>0.02166454397363704</v>
       </c>
       <c r="D53" s="5" t="n">
-        <v>0.0002424199977492792</v>
-      </c>
-      <c r="E53" s="5" t="n">
-        <v>0.004506537112968475</v>
+        <v>0.0449824981561958</v>
+      </c>
+      <c r="E53" s="4" t="n">
+        <v>-0.01007422180378171</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -79699,7 +79663,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-28_2025-06-03</t>
+          <t>2025-06-11_2025-06-17</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -79711,20 +79675,29 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>KAB. SINJAI</t>
-        </is>
-      </c>
-      <c r="B54" s="6" t="inlineStr"/>
-      <c r="C54" s="4" t="n">
-        <v>-0.03510204925731231</v>
-      </c>
-      <c r="D54" s="6" t="inlineStr"/>
+          <t>KAB. PESISIR BARAT</t>
+        </is>
+      </c>
+      <c r="B54" s="5" t="n">
+        <v>0.110202574420141</v>
+      </c>
+      <c r="C54" s="5" t="n">
+        <v>0.03767220983938128</v>
+      </c>
+      <c r="D54" s="5" t="n">
+        <v>1.696163704626156</v>
+      </c>
       <c r="E54" s="5" t="n">
-        <v>0.1248099424989299</v>
+        <v>1.805049403264653</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2025-06-24_2025-06-30</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -79736,54 +79709,54 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>KAB. SUKAMARA</t>
-        </is>
-      </c>
-      <c r="B55" s="4" t="n">
-        <v>-0.02915347618736483</v>
-      </c>
+          <t>KAB. SAMBAS</t>
+        </is>
+      </c>
+      <c r="B55" s="6" t="inlineStr"/>
       <c r="C55" s="4" t="n">
-        <v>-0.05077667861100533</v>
-      </c>
-      <c r="D55" s="5" t="n">
-        <v>3.490157198201878</v>
-      </c>
+        <v>-0.07023693687968006</v>
+      </c>
+      <c r="D55" s="6" t="inlineStr"/>
       <c r="E55" s="5" t="n">
-        <v>5.850716010200014</v>
+        <v>0.5806279775517019</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-16_2025-05-22</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2025-06-27_2025-07-03</t>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-20_2025-07-26</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>KAB. SUMENEP</t>
-        </is>
-      </c>
-      <c r="B56" s="6" t="inlineStr"/>
+          <t>KAB. SAMPANG</t>
+        </is>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>-0.1343411376228456</v>
+      </c>
       <c r="C56" s="4" t="n">
-        <v>-0.06020185800334003</v>
-      </c>
-      <c r="D56" s="6" t="inlineStr"/>
+        <v>-0.06939344128566347</v>
+      </c>
+      <c r="D56" s="5" t="n">
+        <v>0.187785854895615</v>
+      </c>
       <c r="E56" s="5" t="n">
-        <v>1.404743864687132</v>
+        <v>0.2510251813419085</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2025-07-02_2025-07-08</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -79795,20 +79768,20 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>KAB. TAKALAR</t>
+          <t>KAB. SERANG</t>
         </is>
       </c>
       <c r="B57" s="4" t="n">
-        <v>-0.04142020123564612</v>
+        <v>-0.07504590833602121</v>
       </c>
       <c r="C57" s="4" t="n">
-        <v>-0.1132869880457979</v>
+        <v>-0.05455638576395258</v>
       </c>
       <c r="D57" s="5" t="n">
-        <v>0.02006778043717108</v>
+        <v>0.0002424199977492792</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>0.003529346732881368</v>
+        <v>0.004506537112968475</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -79817,41 +79790,32 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-06-22_2025-06-28</t>
+          <t>2025-05-28_2025-06-03</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-07-13_2025-07-19</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>KAB. TAPANULI SELATAN</t>
-        </is>
-      </c>
-      <c r="B58" s="4" t="n">
-        <v>-0.09331805471631796</v>
-      </c>
+          <t>KAB. SINJAI</t>
+        </is>
+      </c>
+      <c r="B58" s="6" t="inlineStr"/>
       <c r="C58" s="4" t="n">
-        <v>-0.1722606013932612</v>
-      </c>
-      <c r="D58" s="5" t="n">
-        <v>0.1009778618995656</v>
-      </c>
+        <v>-0.03510204925731231</v>
+      </c>
+      <c r="D58" s="6" t="inlineStr"/>
       <c r="E58" s="5" t="n">
-        <v>0.557630085105139</v>
+        <v>0.1248099424989299</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>2025-06-18_2025-06-24</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -79863,20 +79827,29 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>KAB. TAPANULI TENGAH</t>
+          <t>KAB. SUKAMARA</t>
         </is>
       </c>
       <c r="B59" s="4" t="n">
-        <v>-0.0888667462517899</v>
+        <v>-0.02915347618736483</v>
       </c>
       <c r="C59" s="4" t="n">
-        <v>-0.1551149414659325</v>
-      </c>
-      <c r="D59" s="6" t="inlineStr"/>
-      <c r="E59" s="6" t="inlineStr"/>
+        <v>-0.05077667861100533</v>
+      </c>
+      <c r="D59" s="5" t="n">
+        <v>3.490157198201878</v>
+      </c>
+      <c r="E59" s="5" t="n">
+        <v>5.850716010200014</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-05-16_2025-05-22</t>
+        </is>
+      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-07-01_2025-07-07</t>
+          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -79888,29 +79861,20 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>KAB. TEMANGGUNG</t>
-        </is>
-      </c>
-      <c r="B60" s="4" t="n">
-        <v>-0.119582243827964</v>
-      </c>
+          <t>KAB. SUMENEP</t>
+        </is>
+      </c>
+      <c r="B60" s="6" t="inlineStr"/>
       <c r="C60" s="4" t="n">
-        <v>-0.1151423872737247</v>
-      </c>
-      <c r="D60" s="4" t="n">
-        <v>-0.01548298132215951</v>
-      </c>
+        <v>-0.06020185800334003</v>
+      </c>
+      <c r="D60" s="6" t="inlineStr"/>
       <c r="E60" s="5" t="n">
-        <v>0.004633742117707856</v>
+        <v>1.404743864687132</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2025-07-15_2025-07-21</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -79922,20 +79886,20 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>KAB. WONOGIRI</t>
+          <t>KAB. TAKALAR</t>
         </is>
       </c>
       <c r="B61" s="4" t="n">
-        <v>-0.08778348317979959</v>
+        <v>-0.04142020123564612</v>
       </c>
       <c r="C61" s="4" t="n">
-        <v>-0.08854594587054952</v>
+        <v>-0.1132869880457979</v>
       </c>
       <c r="D61" s="5" t="n">
-        <v>0.135084091029001</v>
+        <v>0.02006778043717108</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>0.1534815017810605</v>
+        <v>0.003529346732881368</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -79944,32 +79908,32 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-07-16_2025-07-22</t>
+          <t>2025-06-22_2025-06-28</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-13_2025-07-19</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>KOTA BANJARBARU</t>
+          <t>KAB. TAPANULI SELATAN</t>
         </is>
       </c>
       <c r="B62" s="4" t="n">
-        <v>-0.1230810439543908</v>
+        <v>-0.09331805471631796</v>
       </c>
       <c r="C62" s="4" t="n">
-        <v>-0.04035281755720881</v>
-      </c>
-      <c r="D62" s="4" t="n">
-        <v>-0.1532249320557131</v>
+        <v>-0.1722606013932612</v>
+      </c>
+      <c r="D62" s="5" t="n">
+        <v>0.1009778618995656</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>0.05756097210478757</v>
+        <v>0.557630085105139</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -79978,7 +79942,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-07-04_2025-07-10</t>
+          <t>2025-06-18_2025-06-24</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -79990,29 +79954,20 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>KOTA DEPOK</t>
-        </is>
-      </c>
-      <c r="B63" s="5" t="n">
-        <v>0.03455113671863309</v>
-      </c>
-      <c r="C63" s="5" t="n">
-        <v>0.02835354651325127</v>
-      </c>
-      <c r="D63" s="5" t="n">
-        <v>0.07704617612777169</v>
-      </c>
-      <c r="E63" s="5" t="n">
-        <v>0.04266505375259059</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
+          <t>KAB. TAPANULI TENGAH</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="n">
+        <v>-0.0888667462517899</v>
+      </c>
+      <c r="C63" s="4" t="n">
+        <v>-0.1551149414659325</v>
+      </c>
+      <c r="D63" s="6" t="inlineStr"/>
+      <c r="E63" s="6" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-06-26_2025-07-02</t>
+          <t>2025-07-01_2025-07-07</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -80024,20 +79979,20 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>KOTA JAKARTA BARAT</t>
-        </is>
-      </c>
-      <c r="B64" s="5" t="n">
-        <v>0.0002190145113004557</v>
-      </c>
-      <c r="C64" s="5" t="n">
-        <v>0.02493519644055735</v>
-      </c>
-      <c r="D64" s="5" t="n">
-        <v>0.03952821330547174</v>
+          <t>KAB. TEMANGGUNG</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="n">
+        <v>-0.119582243827964</v>
+      </c>
+      <c r="C64" s="4" t="n">
+        <v>-0.1151423872737247</v>
+      </c>
+      <c r="D64" s="4" t="n">
+        <v>-0.01548298132215951</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>0.03646160133862484</v>
+        <v>0.004633742117707856</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -80046,7 +80001,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-06-27_2025-07-03</t>
+          <t>2025-07-15_2025-07-21</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -80058,20 +80013,20 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>KOTA JAKARTA PUSAT</t>
-        </is>
-      </c>
-      <c r="B65" s="5" t="n">
-        <v>0.004346010737160858</v>
-      </c>
-      <c r="C65" s="5" t="n">
-        <v>0.05230131727818127</v>
+          <t>KAB. WONOGIRI</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="n">
+        <v>-0.08778348317979959</v>
+      </c>
+      <c r="C65" s="4" t="n">
+        <v>-0.08854594587054952</v>
       </c>
       <c r="D65" s="5" t="n">
-        <v>0.05515273798791069</v>
+        <v>0.135084091029001</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>0.06385712655046465</v>
+        <v>0.1534815017810605</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -80080,7 +80035,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-06-29_2025-07-05</t>
+          <t>2025-07-16_2025-07-22</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -80092,20 +80047,20 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>KOTA JAKARTA SELATAN</t>
-        </is>
-      </c>
-      <c r="B66" s="5" t="n">
-        <v>0.4337636784930454</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>0.5224238334963245</v>
-      </c>
-      <c r="D66" s="5" t="n">
-        <v>0.02158738783875887</v>
+          <t>KOTA BANJARBARU</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="n">
+        <v>-0.1230810439543908</v>
+      </c>
+      <c r="C66" s="4" t="n">
+        <v>-0.04035281755720881</v>
+      </c>
+      <c r="D66" s="4" t="n">
+        <v>-0.1532249320557131</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>0.03422353185597929</v>
+        <v>0.05756097210478757</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -80114,32 +80069,32 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-06-26_2025-07-02</t>
+          <t>2025-07-04_2025-07-10</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-07-18_2025-07-24</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>KOTA JAKARTA TIMUR</t>
+          <t>KOTA DEPOK</t>
         </is>
       </c>
       <c r="B67" s="5" t="n">
-        <v>0.01178938639379902</v>
+        <v>0.03455113671863309</v>
       </c>
       <c r="C67" s="5" t="n">
-        <v>0.02346760540446283</v>
+        <v>0.02835354651325127</v>
       </c>
       <c r="D67" s="5" t="n">
-        <v>0.03639794017388245</v>
+        <v>0.07704617612777169</v>
       </c>
       <c r="E67" s="5" t="n">
-        <v>0.04081924424601425</v>
+        <v>0.04266505375259059</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -80148,7 +80103,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-06-27_2025-07-03</t>
+          <t>2025-06-26_2025-07-02</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -80160,20 +80115,29 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>KOTA JAKARTA UTARA</t>
-        </is>
-      </c>
-      <c r="B68" s="6" t="inlineStr"/>
+          <t>KOTA JAKARTA BARAT</t>
+        </is>
+      </c>
+      <c r="B68" s="5" t="n">
+        <v>0.0002190145113004557</v>
+      </c>
       <c r="C68" s="5" t="n">
-        <v>0.05556976705496127</v>
-      </c>
-      <c r="D68" s="6" t="inlineStr"/>
+        <v>0.02493519644055735</v>
+      </c>
+      <c r="D68" s="5" t="n">
+        <v>0.03952821330547174</v>
+      </c>
       <c r="E68" s="5" t="n">
-        <v>0.07654351987653694</v>
+        <v>0.03646160133862484</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -80185,47 +80149,54 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>KOTA KENDARI</t>
-        </is>
-      </c>
-      <c r="B69" s="4" t="n">
-        <v>-0.05906724544304733</v>
-      </c>
-      <c r="C69" s="4" t="n">
-        <v>-0.08902151898329733</v>
-      </c>
-      <c r="D69" s="6" t="inlineStr"/>
+          <t>KOTA JAKARTA PUSAT</t>
+        </is>
+      </c>
+      <c r="B69" s="5" t="n">
+        <v>0.004346010737160858</v>
+      </c>
+      <c r="C69" s="5" t="n">
+        <v>0.05230131727818127</v>
+      </c>
+      <c r="D69" s="5" t="n">
+        <v>0.05515273798791069</v>
+      </c>
       <c r="E69" s="5" t="n">
-        <v>31.21142788981194</v>
+        <v>0.06385712655046465</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-13_2025-05-19</t>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2025-06-29_2025-07-05</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-07-11_2025-07-17</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>KOTA LANGSA</t>
-        </is>
-      </c>
-      <c r="B70" s="4" t="n">
-        <v>-0.5031930091564516</v>
-      </c>
-      <c r="C70" s="4" t="n">
-        <v>-0.09325212102695012</v>
+          <t>KOTA JAKARTA SELATAN</t>
+        </is>
+      </c>
+      <c r="B70" s="5" t="n">
+        <v>0.4337636784930454</v>
+      </c>
+      <c r="C70" s="5" t="n">
+        <v>0.5224238334963245</v>
       </c>
       <c r="D70" s="5" t="n">
-        <v>2.704461950457083</v>
+        <v>0.02158738783875887</v>
       </c>
       <c r="E70" s="5" t="n">
-        <v>4.390505684462563</v>
+        <v>0.03422353185597929</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -80234,32 +80205,32 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-06-15_2025-06-21</t>
+          <t>2025-06-26_2025-07-02</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-18_2025-07-24</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>KOTA MAKASSAR</t>
-        </is>
-      </c>
-      <c r="B71" s="4" t="n">
-        <v>-0.008727675815067617</v>
-      </c>
-      <c r="C71" s="4" t="n">
-        <v>-0.06157877308665385</v>
-      </c>
-      <c r="D71" s="4" t="n">
-        <v>-0.01782217840818711</v>
-      </c>
-      <c r="E71" s="4" t="n">
-        <v>-0.03514045943803284</v>
+          <t>KOTA JAKARTA TIMUR</t>
+        </is>
+      </c>
+      <c r="B71" s="5" t="n">
+        <v>0.01178938639379902</v>
+      </c>
+      <c r="C71" s="5" t="n">
+        <v>0.02346760540446283</v>
+      </c>
+      <c r="D71" s="5" t="n">
+        <v>0.03639794017388245</v>
+      </c>
+      <c r="E71" s="5" t="n">
+        <v>0.04081924424601425</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -80268,7 +80239,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-06-22_2025-06-28</t>
+          <t>2025-06-27_2025-07-03</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -80280,79 +80251,81 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>KOTA MATARAM</t>
+          <t>KOTA JAKARTA UTARA</t>
         </is>
       </c>
       <c r="B72" s="6" t="inlineStr"/>
-      <c r="C72" s="4" t="n">
-        <v>-0.1474976595150131</v>
+      <c r="C72" s="5" t="n">
+        <v>0.05556976705496127</v>
       </c>
       <c r="D72" s="6" t="inlineStr"/>
-      <c r="E72" s="4" t="n">
-        <v>-0.2168845137306823</v>
+      <c r="E72" s="5" t="n">
+        <v>0.07654351987653694</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-18_2025-05-24</t>
+          <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-07-18_2025-07-24</t>
+          <t>2025-07-24_2025-07-30</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>KOTA PADANGSIDIMPUAN</t>
+          <t>KOTA KENDARI</t>
         </is>
       </c>
       <c r="B73" s="4" t="n">
-        <v>-0.06028739524223507</v>
+        <v>-0.05906724544304733</v>
       </c>
       <c r="C73" s="4" t="n">
-        <v>-0.1318820446890598</v>
-      </c>
-      <c r="D73" s="5" t="n">
-        <v>0.4053639748453003</v>
-      </c>
+        <v>-0.08902151898329733</v>
+      </c>
+      <c r="D73" s="6" t="inlineStr"/>
       <c r="E73" s="5" t="n">
-        <v>0.7437573049514561</v>
+        <v>31.21142788981194</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2025-06-18_2025-06-24</t>
+          <t>2025-05-13_2025-05-19</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-11_2025-07-17</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>KOTA PAGAR ALAM</t>
-        </is>
-      </c>
-      <c r="B74" s="6" t="inlineStr"/>
+          <t>KOTA LANGSA</t>
+        </is>
+      </c>
+      <c r="B74" s="4" t="n">
+        <v>-0.5031930091564516</v>
+      </c>
       <c r="C74" s="4" t="n">
-        <v>-0.0375794172878199</v>
-      </c>
-      <c r="D74" s="6" t="inlineStr"/>
-      <c r="E74" s="4" t="n">
-        <v>-0.001795254701171753</v>
+        <v>-0.09325212102695012</v>
+      </c>
+      <c r="D74" s="5" t="n">
+        <v>2.704461950457083</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>4.390505684462563</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2025-06-15_2025-06-21</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -80364,29 +80337,20 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>KOTA PAYAKUMBUH</t>
-        </is>
-      </c>
-      <c r="B75" s="5" t="n">
-        <v>0.008446508035029743</v>
-      </c>
+          <t>KOTA LUBUK LINGGAU</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr"/>
       <c r="C75" s="5" t="n">
-        <v>0.01510042875907942</v>
-      </c>
-      <c r="D75" s="4" t="n">
-        <v>-0.09199075289844323</v>
-      </c>
-      <c r="E75" s="4" t="n">
-        <v>-0.1076491181974275</v>
+        <v>0.004849634347143945</v>
+      </c>
+      <c r="D75" s="6" t="inlineStr"/>
+      <c r="E75" s="5" t="n">
+        <v>0.1144849444008561</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>2025-06-22_2025-06-28</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -80398,20 +80362,20 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>KOTA PONTIANAK</t>
+          <t>KOTA MAKASSAR</t>
         </is>
       </c>
       <c r="B76" s="4" t="n">
-        <v>-0.1132666357818837</v>
+        <v>-0.008727675815067617</v>
       </c>
       <c r="C76" s="4" t="n">
-        <v>-0.1198283777234519</v>
+        <v>-0.06157877308665385</v>
       </c>
       <c r="D76" s="4" t="n">
-        <v>-0.004769700577166017</v>
-      </c>
-      <c r="E76" s="5" t="n">
-        <v>0.0559274519973221</v>
+        <v>-0.01782217840818711</v>
+      </c>
+      <c r="E76" s="4" t="n">
+        <v>-0.03514045943803284</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -80420,7 +80384,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-07-02_2025-07-08</t>
+          <t>2025-06-22_2025-06-28</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -80432,54 +80396,54 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>KOTA PRABUMULIH</t>
-        </is>
-      </c>
-      <c r="B77" s="4" t="n">
-        <v>-0.01798870228259308</v>
-      </c>
+          <t>KOTA MATARAM</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr"/>
       <c r="C77" s="4" t="n">
-        <v>-0.03707988343396532</v>
-      </c>
-      <c r="D77" s="5" t="n">
-        <v>0.006216456898238091</v>
-      </c>
+        <v>-0.1474976595150131</v>
+      </c>
+      <c r="D77" s="6" t="inlineStr"/>
       <c r="E77" s="4" t="n">
-        <v>-0.01609098488529392</v>
+        <v>-0.2168845137306823</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>2025-07-19_2025-07-25</t>
+          <t>2025-05-18_2025-05-24</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-07-24_2025-07-30</t>
+          <t>2025-07-18_2025-07-24</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>KOTA SAMARINDA</t>
-        </is>
-      </c>
-      <c r="B78" s="6" t="inlineStr"/>
-      <c r="C78" s="5" t="n">
-        <v>0.01619987386278914</v>
-      </c>
-      <c r="D78" s="6" t="inlineStr"/>
+          <t>KOTA PADANGSIDIMPUAN</t>
+        </is>
+      </c>
+      <c r="B78" s="4" t="n">
+        <v>-0.06028739524223507</v>
+      </c>
+      <c r="C78" s="4" t="n">
+        <v>-0.1318820446890598</v>
+      </c>
+      <c r="D78" s="5" t="n">
+        <v>0.4053639748453003</v>
+      </c>
       <c r="E78" s="5" t="n">
-        <v>0.1014644444642722</v>
+        <v>0.7437573049514561</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2025-06-18_2025-06-24</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -80491,29 +80455,20 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>KOTA SIBOLGA</t>
-        </is>
-      </c>
-      <c r="B79" s="4" t="n">
-        <v>-0.1788950911871061</v>
-      </c>
+          <t>KOTA PAGAR ALAM</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr"/>
       <c r="C79" s="4" t="n">
-        <v>-0.1471700388842455</v>
-      </c>
-      <c r="D79" s="5" t="n">
-        <v>0.1203391600404973</v>
-      </c>
-      <c r="E79" s="5" t="n">
-        <v>0.05933295058933344</v>
+        <v>-0.0375794172878199</v>
+      </c>
+      <c r="D79" s="6" t="inlineStr"/>
+      <c r="E79" s="4" t="n">
+        <v>-0.001795254701171753</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>2025-07-04_2025-07-10</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -80525,23 +80480,209 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>KOTA PAYAKUMBUH</t>
+        </is>
+      </c>
+      <c r="B80" s="5" t="n">
+        <v>0.008446508035029743</v>
+      </c>
+      <c r="C80" s="5" t="n">
+        <v>0.01510042875907942</v>
+      </c>
+      <c r="D80" s="4" t="n">
+        <v>-0.09199075289844323</v>
+      </c>
+      <c r="E80" s="4" t="n">
+        <v>-0.1076491181974275</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2025-06-22_2025-06-28</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2025-07-24_2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>KOTA PONTIANAK</t>
+        </is>
+      </c>
+      <c r="B81" s="4" t="n">
+        <v>-0.1132666357818837</v>
+      </c>
+      <c r="C81" s="4" t="n">
+        <v>-0.1198283777234519</v>
+      </c>
+      <c r="D81" s="4" t="n">
+        <v>-0.004769700577166017</v>
+      </c>
+      <c r="E81" s="5" t="n">
+        <v>0.0559274519973221</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2025-07-02_2025-07-08</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2025-07-24_2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>KOTA PRABUMULIH</t>
+        </is>
+      </c>
+      <c r="B82" s="4" t="n">
+        <v>-0.01798870228259308</v>
+      </c>
+      <c r="C82" s="4" t="n">
+        <v>-0.03707988343396532</v>
+      </c>
+      <c r="D82" s="5" t="n">
+        <v>0.006216456898238091</v>
+      </c>
+      <c r="E82" s="4" t="n">
+        <v>-0.01609098488529392</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2025-07-19_2025-07-25</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2025-07-24_2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>KOTA SAMARINDA</t>
+        </is>
+      </c>
+      <c r="B83" s="6" t="inlineStr"/>
+      <c r="C83" s="5" t="n">
+        <v>0.01619987386278914</v>
+      </c>
+      <c r="D83" s="6" t="inlineStr"/>
+      <c r="E83" s="5" t="n">
+        <v>0.1014644444642722</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2025-07-24_2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>KOTA SEMARANG</t>
+        </is>
+      </c>
+      <c r="B84" s="6" t="inlineStr"/>
+      <c r="C84" s="4" t="n">
+        <v>-0.005733715116890886</v>
+      </c>
+      <c r="D84" s="6" t="inlineStr"/>
+      <c r="E84" s="5" t="n">
+        <v>0.02064518403546907</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2025-07-24_2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>KOTA SIBOLGA</t>
+        </is>
+      </c>
+      <c r="B85" s="4" t="n">
+        <v>-0.1788950911871061</v>
+      </c>
+      <c r="C85" s="4" t="n">
+        <v>-0.1471700388842455</v>
+      </c>
+      <c r="D85" s="5" t="n">
+        <v>0.1203391600404973</v>
+      </c>
+      <c r="E85" s="5" t="n">
+        <v>0.05933295058933344</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>2025-05-11_2025-05-17</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2025-07-04_2025-07-10</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2025-07-24_2025-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
           <t>KOTA SINGKAWANG</t>
         </is>
       </c>
-      <c r="B80" s="6" t="inlineStr"/>
-      <c r="C80" s="4" t="n">
+      <c r="B86" s="6" t="inlineStr"/>
+      <c r="C86" s="4" t="n">
         <v>-0.06535237837594236</v>
       </c>
-      <c r="D80" s="6" t="inlineStr"/>
-      <c r="E80" s="4" t="n">
+      <c r="D86" s="6" t="inlineStr"/>
+      <c r="E86" s="4" t="n">
         <v>-0.106130993407725</v>
       </c>
-      <c r="F80" t="inlineStr">
+      <c r="F86" t="inlineStr">
         <is>
           <t>2025-05-11_2025-05-17</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr">
+      <c r="H86" t="inlineStr">
         <is>
           <t>2025-07-24_2025-07-30</t>
         </is>

</xml_diff>